<commit_message>
updates to goat and moose transect
</commit_message>
<xml_diff>
--- a/sims/src/observations/goat/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Goat_test.xlsx
+++ b/sims/src/observations/goat/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Goat_test.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/Desktop/BHBC-1412:BHBC-1974/Goat/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/DevelopmentProjects/biohubbc-utils/sims/src/observations/goat/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A265612-BC6F-6A48-B20E-BF97AA490024}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8498436A-4EC1-DF4A-8069-02FD9E9BA24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-18940" yWindow="-20540" windowWidth="23260" windowHeight="12580" tabRatio="672" activeTab="2" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
+    <workbookView xWindow="-17440" yWindow="-20520" windowWidth="25300" windowHeight="13100" tabRatio="672" activeTab="1" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
   </bookViews>
   <sheets>
     <sheet name="Effort &amp; Site Conditions" sheetId="2" r:id="rId1"/>
@@ -1895,7 +1895,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="386">
   <si>
     <t>Date</t>
   </si>
@@ -3050,6 +3050,9 @@
   </si>
   <si>
     <t>marked_comment_2</t>
+  </si>
+  <si>
+    <t>Group Label1</t>
   </si>
 </sst>
 </file>
@@ -4031,7 +4034,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9934F4F-97FC-4CFD-8FF0-86937AF9AE11}">
   <dimension ref="A1:AJ566"/>
   <sheetViews>
-    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+    <sheetView zoomScale="75" zoomScaleNormal="75" workbookViewId="0">
       <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
@@ -17940,8 +17943,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7CACE0D7-C202-416C-A799-EE712DC4F630}">
   <dimension ref="A1:AG501"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="N1" sqref="N1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J1" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.6640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -18004,7 +18007,7 @@
         <v>304</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>291</v>
+        <v>385</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>0</v>
@@ -25731,7 +25734,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B7C5C50-7D41-4386-95DF-AC97EF3E04C6}">
   <dimension ref="A1:M104"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
removed marked_animal_comments from measurementOrFact
</commit_message>
<xml_diff>
--- a/sims/src/observations/goat/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Goat_test.xlsx
+++ b/sims/src/observations/goat/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/Goat_test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/anissa/DevelopmentProjects/biohubbc-utils/sims/src/observations/goat/aerial-population-total-count-recruitment-composition-survey/2.1/test-data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8498436A-4EC1-DF4A-8069-02FD9E9BA24E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE201205-7535-4D45-8D6C-23DEE72677A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-17440" yWindow="-20520" windowWidth="25300" windowHeight="13100" tabRatio="672" activeTab="1" xr2:uid="{EA928297-87AF-4A2F-92BD-649BD8B345BB}"/>
   </bookViews>
@@ -748,19 +748,38 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-A unique identification label assigned to track a group of animals detected during the course of a Block Visit, e.g., G25. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">A unique identification label assigned to track a group of animals detected during the course of a Block Visit, e.g., G25. 
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
 </t>
         </r>
         <r>
           <rPr>
             <u/>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
@@ -769,13 +788,51 @@
         <r>
           <rPr>
             <sz val="9"/>
-            <color indexed="81"/>
+            <color rgb="FF000000"/>
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
           <t xml:space="preserve">
-INSTRUCTIONS: Labels should contain letters, start with a character other than zero, and contain no hyphens. For example, 'AM330' or 'D30' will work well with Excel.
-Avoid Labels that do not contain letters, begin with zero, or contain hyphens. For example, avoid '003' or '2-5', because Excel may automatically reformat such data</t>
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">INSTRUCTIONS: Labels should contain letters, start with a character other than zero, and contain no hyphens. For example, 'AM330' or 'D30' will work well with Excel.
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color rgb="FF000000"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Avoid Labels that do not contain letters, begin with zero, or contain hyphens. For example, avoid '003' or '2-5', because Excel may automatically reformat such data</t>
         </r>
       </text>
     </comment>
@@ -1895,7 +1952,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="386">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="441" uniqueCount="385">
   <si>
     <t>Date</t>
   </si>
@@ -3050,9 +3107,6 @@
   </si>
   <si>
     <t>marked_comment_2</t>
-  </si>
-  <si>
-    <t>Group Label1</t>
   </si>
 </sst>
 </file>
@@ -18007,7 +18061,7 @@
         <v>304</v>
       </c>
       <c r="J1" s="16" t="s">
-        <v>385</v>
+        <v>291</v>
       </c>
       <c r="K1" s="15" t="s">
         <v>0</v>

</xml_diff>